<commit_message>
Send email: Total score
</commit_message>
<xml_diff>
--- a/xlsx-template/attch-email.xlsx
+++ b/xlsx-template/attch-email.xlsx
@@ -66,7 +66,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +77,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -103,12 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -117,6 +121,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -399,50 +410,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="26.28515625" customWidth="1"/>
     <col min="8" max="8" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1"/>
@@ -450,21 +461,40 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>